<commit_message>
Rules de problema abstracto a solucion abstracta (intento)
</commit_message>
<xml_diff>
--- a/sbc/Practica2.xlsx
+++ b/sbc/Practica2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,11 +13,16 @@
     <sheet name="Hoja3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="92">
   <si>
     <t>Ejercicios</t>
   </si>
@@ -28,6 +33,9 @@
     <t>Dificultad</t>
   </si>
   <si>
+    <t>Prioridad(1-max, 2…)</t>
+  </si>
+  <si>
     <t>Pecho (Pesas)</t>
   </si>
   <si>
@@ -43,60 +51,63 @@
     <t>Press Banca</t>
   </si>
   <si>
+    <t>P, M</t>
+  </si>
+  <si>
+    <t>Musculación:</t>
+  </si>
+  <si>
+    <t>ns*(90s+(ºintens)s+nr*3)</t>
+  </si>
+  <si>
+    <t>3x8-10</t>
+  </si>
+  <si>
+    <t>Movimiento lento, 80% RM</t>
+  </si>
+  <si>
+    <t>Press Banca inclinado</t>
+  </si>
+  <si>
+    <t>Resistencia:</t>
+  </si>
+  <si>
+    <t>ns*(45s+(ºintens)s+nr*2)</t>
+  </si>
+  <si>
+    <t>4x12-15</t>
+  </si>
+  <si>
+    <t>Movimiento explosivo, 55% RM</t>
+  </si>
+  <si>
+    <t>Press Banca Declinado</t>
+  </si>
+  <si>
+    <t>Fuerza:</t>
+  </si>
+  <si>
+    <t>ns*(150s+(ºintens)s+nr*4)</t>
+  </si>
+  <si>
+    <t>5x4-6</t>
+  </si>
+  <si>
+    <t>Movimento completo, 90% RM</t>
+  </si>
+  <si>
+    <t>Aperturas Planas</t>
+  </si>
+  <si>
+    <t>Equilibrio</t>
+  </si>
+  <si>
+    <t>Pullover</t>
+  </si>
+  <si>
     <t>P</t>
   </si>
   <si>
-    <t>Musculación:</t>
-  </si>
-  <si>
-    <t>ns*(90s+(ºintens)s+nr*3)</t>
-  </si>
-  <si>
-    <t>3x8-10</t>
-  </si>
-  <si>
-    <t>Movimiento lento, 80% RM</t>
-  </si>
-  <si>
-    <t>Press Banca inclinado</t>
-  </si>
-  <si>
-    <t>Resistencia:</t>
-  </si>
-  <si>
-    <t>ns*(45s+(ºintens)s+nr*2)</t>
-  </si>
-  <si>
-    <t>4x12-15</t>
-  </si>
-  <si>
-    <t>Movimiento explosivo, 55% RM</t>
-  </si>
-  <si>
-    <t>Press Banca Declinado</t>
-  </si>
-  <si>
-    <t>Fuerza:</t>
-  </si>
-  <si>
-    <t>ns*(150s+(ºintens)s+nr*4)</t>
-  </si>
-  <si>
-    <t>5x4-6</t>
-  </si>
-  <si>
-    <t>Movimento completo, 90% RM</t>
-  </si>
-  <si>
-    <t>Aperturas Planas</t>
-  </si>
-  <si>
-    <t>Equilibrio</t>
-  </si>
-  <si>
-    <t>Pullover</t>
-  </si>
-  <si>
     <t>Flexibilidad</t>
   </si>
   <si>
@@ -106,37 +117,40 @@
     <t>Fondos </t>
   </si>
   <si>
+    <t>P, NP</t>
+  </si>
+  <si>
+    <t>Flexiones</t>
+  </si>
+  <si>
+    <t>Espalda (Polea)</t>
+  </si>
+  <si>
+    <t>Polea tras-nuca</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Polea al pecho</t>
+  </si>
+  <si>
+    <t>Jalones al pecho</t>
+  </si>
+  <si>
+    <t>Remo</t>
+  </si>
+  <si>
+    <t>Remo sentado</t>
+  </si>
+  <si>
+    <t>Espalda (Barra)</t>
+  </si>
+  <si>
+    <t>Fat-man Pullups</t>
+  </si>
+  <si>
     <t>NP</t>
-  </si>
-  <si>
-    <t>Flexiones</t>
-  </si>
-  <si>
-    <t>Espalda (Polea)</t>
-  </si>
-  <si>
-    <t>Polea tras-nuca</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>Polea al pecho</t>
-  </si>
-  <si>
-    <t>Jalones al pecho</t>
-  </si>
-  <si>
-    <t>Remo</t>
-  </si>
-  <si>
-    <t>Remo sentado</t>
-  </si>
-  <si>
-    <t>Espalda (Barra)</t>
-  </si>
-  <si>
-    <t>Fat-man Pullups</t>
   </si>
   <si>
     <t>Dominadas abiertas</t>
@@ -396,17 +410,17 @@
   <dimension ref="A1:K64"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.8622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="10.7295918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.3214285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.7602040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.19897959183674"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.7295918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1012145748988"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="10.8178137651822"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.21457489878543"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.8178137651822"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -419,538 +433,658 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="G4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="D5" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="G5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D6" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="G6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D7" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="G7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D8" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="G8" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="C15" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="D16" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="D20" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="D21" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="D27" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="D28" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="D32" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D34" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="D36" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="D38" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D39" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C41" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D41" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C42" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D42" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="D46" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B47" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="C47" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C49" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D49" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>1</v>
@@ -958,10 +1092,10 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C52" s="0" t="n">
         <v>1</v>
@@ -969,10 +1103,10 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C53" s="0" t="n">
         <v>1</v>
@@ -980,10 +1114,10 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C54" s="0" t="n">
         <v>1</v>
@@ -991,10 +1125,10 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C55" s="0" t="n">
         <v>1</v>
@@ -1002,83 +1136,101 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1105,7 +1257,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.8178137651822"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1131,7 +1283,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.8178137651822"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>